<commit_message>
Atualização de porgresso e novos requisitos
</commit_message>
<xml_diff>
--- a/Backlog de requisitos/Backlog de requisitos.xlsx
+++ b/Backlog de requisitos/Backlog de requisitos.xlsx
@@ -1,32 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projeto pessoal\Backlog de requisitos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\OneDrive\Ambiente de Trabalho\Paulo\FIFA CONNECTION\FIFA_CONNECTION\Backlog de requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328210C9-1660-4753-9190-CA5C46F85759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591A1F6A-C648-4050-B489-B979103D4E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Burndown " sheetId="2" r:id="rId2"/>
+    <sheet name="Gráficos para documentação " sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="70">
   <si>
     <t>Requisito</t>
   </si>
@@ -224,6 +239,18 @@
   </si>
   <si>
     <t xml:space="preserve">Gráfico de progresso atual </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Docuemntação </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criação de um documento detalhando cada etapa, com a finalidade de padronizar e dar continuidade ao projeto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ano </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendas </t>
   </si>
 </sst>
 </file>
@@ -405,32 +432,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -454,17 +471,33 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="34">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -478,12 +511,13 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0"/>
+          <bgColor rgb="FF1B1D1E"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -497,36 +531,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Bahnschrift SemiBold Condensed"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF1B1D1E"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -834,6 +838,72 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Bahnschrift SemiBold Condensed"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF1B1D1E"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1021,19 +1091,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>197</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>157</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>117</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>77</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1509,10 +1579,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>197</c:v>
+                  <c:v>171</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1618,6 +1688,363 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800">
+                <a:latin typeface="Bahnschrift SemiBold SemiConden" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Vendas</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]Planilha1!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vendas </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="E0B740"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]Planilha1!$C$4:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2023</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]Planilha1!$D$4:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>12000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13749542.640000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15804072</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18165600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20880000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27120000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30645600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34629528</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39131366</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44218444</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FB20-4013-9743-3F153CB926A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="290132336"/>
+        <c:axId val="290132816"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="290132336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="290132816"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="290132816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="290132336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="28575" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:srgbClr val="1B1D1E"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1695,6 +2122,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2388,6 +2855,511 @@
       <cs:styleClr val="auto"/>
     </cs:lnRef>
     <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -2780,142 +3752,6 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3729311</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>186426</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>84597</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>183624</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Retângulo: Único Canto Arredondado 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B7474E5-784F-4C04-8251-1775323547F9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5107635" y="186426"/>
-          <a:ext cx="535080" cy="389404"/>
-        </a:xfrm>
-        <a:prstGeom prst="round1Rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="1B1D1E"/>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="1B1D1E"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="pt-BR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3729311</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>369794</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>84597</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>183624</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Retângulo: Único Canto Arredondado 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A415E5F-687D-4A8C-9558-FA8BE47AA19D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5107635" y="6925235"/>
-          <a:ext cx="535080" cy="385330"/>
-        </a:xfrm>
-        <a:prstGeom prst="round1Rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="1B1D1E"/>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="1B1D1E"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="pt-BR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
@@ -3066,74 +3902,6 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3729311</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>369794</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>84597</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>183624</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="Retângulo: Único Canto Arredondado 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FF0415B-2249-4E11-9935-F24D737AF7A5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5107635" y="6925235"/>
-          <a:ext cx="535080" cy="385330"/>
-        </a:xfrm>
-        <a:prstGeom prst="round1Rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="1B1D1E"/>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="1B1D1E"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="pt-BR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
@@ -3416,9 +4184,166 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD9C386C-D847-402A-9E2F-2F0BEC40B075}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Product backlog"/>
+      <sheetName val="Burndown "/>
+      <sheetName val="Planilha1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="3">
+          <cell r="D3" t="str">
+            <v xml:space="preserve">Vendas </v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="C4">
+            <v>2013</v>
+          </cell>
+          <cell r="D4">
+            <v>12000000</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="C5">
+            <v>2014</v>
+          </cell>
+          <cell r="D5">
+            <v>13749542.640000001</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="C6">
+            <v>2015</v>
+          </cell>
+          <cell r="D6">
+            <v>15804072</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>2016</v>
+          </cell>
+          <cell r="D7">
+            <v>18165600</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8">
+            <v>2017</v>
+          </cell>
+          <cell r="D8">
+            <v>20880000</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="C9">
+            <v>2018</v>
+          </cell>
+          <cell r="D9">
+            <v>24000000</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="C10">
+            <v>2019</v>
+          </cell>
+          <cell r="D10">
+            <v>27120000</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>2020</v>
+          </cell>
+          <cell r="D11">
+            <v>30645600</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>2021</v>
+          </cell>
+          <cell r="D12">
+            <v>34629528</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="C13">
+            <v>2022</v>
+          </cell>
+          <cell r="D13">
+            <v>39131366</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="C14">
+            <v>2023</v>
+          </cell>
+          <cell r="D14">
+            <v>44218444</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{44AF3545-DDD6-4C1E-9F55-A4508074C594}" name="Tabela1" displayName="Tabela1" ref="B4:F17" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27">
-  <autoFilter ref="B4:F17" xr:uid="{44AF3545-DDD6-4C1E-9F55-A4508074C594}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{44AF3545-DDD6-4C1E-9F55-A4508074C594}" name="Tabela1" displayName="Tabela1" ref="B4:F18" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" tableBorderDxfId="25">
+  <autoFilter ref="B4:F18" xr:uid="{44AF3545-DDD6-4C1E-9F55-A4508074C594}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -3426,18 +4351,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{400CD48F-1C3A-4A69-89EF-43CB9D29EC0A}" name="Requisito" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{B397096E-5AAB-4811-9398-F4AE59744432}" name="Descrição " dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{0B982FCA-EF74-4493-A081-01103E481DF0}" name="Classificação " dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{4A74B25D-BCAC-45DF-BC14-AF7BA5CEF0DC}" name="Tamanho " dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{40F4E805-30D6-408F-9B3F-FD6CC6CF73E5}" name="Fibonacci " dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{400CD48F-1C3A-4A69-89EF-43CB9D29EC0A}" name="Requisito" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{B397096E-5AAB-4811-9398-F4AE59744432}" name="Descrição " dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{0B982FCA-EF74-4493-A081-01103E481DF0}" name="Classificação " dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{4A74B25D-BCAC-45DF-BC14-AF7BA5CEF0DC}" name="Tamanho " dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{40F4E805-30D6-408F-9B3F-FD6CC6CF73E5}" name="Fibonacci " dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D6703F94-6384-438B-B7D0-BE88CB44C8BC}" name="Tabela13" displayName="Tabela13" ref="B23:F29" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" tableBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D6703F94-6384-438B-B7D0-BE88CB44C8BC}" name="Tabela13" displayName="Tabela13" ref="B23:F29" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17">
   <autoFilter ref="B23:F29" xr:uid="{D6703F94-6384-438B-B7D0-BE88CB44C8BC}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3446,18 +4371,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3CD53ACE-5C58-4A29-896A-F4FCB3C9822B}" name="Requisito" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{4E4BC438-43C5-40C1-B4E1-CB9D2C6DED80}" name="Descrição " dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{FE25C7CB-7C4E-4DF5-BAED-D4E3D37A63A5}" name="Classificação " dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{082E7397-FEFD-4DE2-AA73-4E7A6D622789}" name="Tamanho " dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{16B2F14C-FCDA-40DC-B8A8-957DE19C7E24}" name="Fibonacci " dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{3CD53ACE-5C58-4A29-896A-F4FCB3C9822B}" name="Requisito" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{4E4BC438-43C5-40C1-B4E1-CB9D2C6DED80}" name="Descrição " dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{FE25C7CB-7C4E-4DF5-BAED-D4E3D37A63A5}" name="Classificação " dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{082E7397-FEFD-4DE2-AA73-4E7A6D622789}" name="Tamanho " dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{16B2F14C-FCDA-40DC-B8A8-957DE19C7E24}" name="Fibonacci " dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BABECFD4-922D-457C-BF20-46F3E2426E3A}" name="Tabela134" displayName="Tabela134" ref="B35:F38" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BABECFD4-922D-457C-BF20-46F3E2426E3A}" name="Tabela134" displayName="Tabela134" ref="B35:F38" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9">
   <autoFilter ref="B35:F38" xr:uid="{BABECFD4-922D-457C-BF20-46F3E2426E3A}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3466,18 +4391,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{65D74C8B-3DBC-425C-A39C-4420AFCE108E}" name="Requisito" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{E1ACF51E-B734-4BB7-AC11-C2B325697F9A}" name="Descrição " dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{318F4AC5-6A64-4007-96AF-D3F98FBFFF6B}" name="Classificação " dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{920893E7-A34A-4ADD-B1FD-669711FBA701}" name="Tamanho " dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{EED2718D-FC2A-47A7-B1C9-E9C2944C7A8A}" name="Fibonacci " dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{65D74C8B-3DBC-425C-A39C-4420AFCE108E}" name="Requisito" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{E1ACF51E-B734-4BB7-AC11-C2B325697F9A}" name="Descrição " dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{318F4AC5-6A64-4007-96AF-D3F98FBFFF6B}" name="Classificação " dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{920893E7-A34A-4ADD-B1FD-669711FBA701}" name="Tamanho " dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{EED2718D-FC2A-47A7-B1C9-E9C2944C7A8A}" name="Fibonacci " dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7EFB2BB2-A11A-49DA-9880-DFE209BF99C4}" name="Tabela4" displayName="Tabela4" ref="B6:E12" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7EFB2BB2-A11A-49DA-9880-DFE209BF99C4}" name="Tabela4" displayName="Tabela4" ref="B6:E12" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="B6:E12" xr:uid="{7EFB2BB2-A11A-49DA-9880-DFE209BF99C4}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3485,12 +4410,26 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{27AD9885-4AD0-4E04-B005-9E75595DBB96}" name="Total de pontos " dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{36E76CE8-0212-48F0-82D4-EB4735F79C0C}" name="Semana" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{08DB7DAC-1C6C-4BEB-AD31-471874B54011}" name="Meta de pontos por semana " dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{2708985B-74EE-42E3-BB5C-8E07804C1C3C}" name="Dias restantes " dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{27AD9885-4AD0-4E04-B005-9E75595DBB96}" name="Total de pontos " dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{36E76CE8-0212-48F0-82D4-EB4735F79C0C}" name="Semana" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{08DB7DAC-1C6C-4BEB-AD31-471874B54011}" name="Meta de pontos por semana " dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{2708985B-74EE-42E3-BB5C-8E07804C1C3C}" name="Dias restantes " dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B97987D1-C440-4454-8C26-F906B4BFEFFD}" name="Tabela5" displayName="Tabela5" ref="B2:C13" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="B2:C13" xr:uid="{B97987D1-C440-4454-8C26-F906B4BFEFFD}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{25E99C69-32F3-49F5-892E-E73C6C958C59}" name="ano " dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{FF482752-02B1-40A5-8AA1-681E5327D50F}" name="Vendas " dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -3759,8 +4698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G52"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C17"/>
+    <sheetView topLeftCell="A29" zoomScale="75" zoomScaleNormal="52" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3774,12 +4713,12 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="8"/>
+      <c r="B3" s="15"/>
     </row>
     <row r="4" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -3800,254 +4739,264 @@
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F17" s="4">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="5" t="s">
+    <row r="18" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="5">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="E18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F18" s="4">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-    </row>
     <row r="19" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
     </row>
     <row r="20" spans="2:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
     </row>
     <row r="21" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="8"/>
+      <c r="B22" s="15"/>
     </row>
     <row r="23" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
@@ -4067,135 +5016,135 @@
       </c>
     </row>
     <row r="24" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="4">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="4">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="4">
         <v>8</v>
       </c>
     </row>
     <row r="27" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F27" s="4">
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F28" s="4">
         <v>8</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F29" s="4">
         <v>8</v>
       </c>
     </row>
     <row r="30" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
     </row>
     <row r="31" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
     </row>
     <row r="32" spans="2:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
     </row>
     <row r="33" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="14" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="34" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="8"/>
+      <c r="B34" s="15"/>
     </row>
     <row r="35" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
@@ -4215,76 +5164,76 @@
       </c>
     </row>
     <row r="36" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E36" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F36" s="5">
+      <c r="F36" s="4">
         <v>8</v>
       </c>
     </row>
     <row r="37" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E37" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F37" s="5">
+      <c r="F37" s="4">
         <v>8</v>
       </c>
     </row>
     <row r="38" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E38" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F38" s="5">
+      <c r="F38" s="4">
         <v>8</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
     </row>
     <row r="40" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
     </row>
     <row r="41" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
     </row>
     <row r="42" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4318,8 +5267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{522AEF28-E0A3-4398-BC6C-55A0E34749B9}">
   <dimension ref="B2:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4336,23 +5285,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="J3" s="19" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="J3" s="17" t="s">
         <v>65</v>
       </c>
       <c r="K3" s="18"/>
@@ -4361,129 +5310,119 @@
       <c r="J4" s="18"/>
       <c r="K4" s="18"/>
     </row>
-    <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-    </row>
+    <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="K6" s="17">
-        <v>197</v>
+      <c r="K6" s="13">
+        <f>B7-K7</f>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="12">
-        <v>197</v>
-      </c>
-      <c r="C7" s="12">
+      <c r="B7" s="8">
+        <v>210</v>
+      </c>
+      <c r="C7" s="8">
         <v>1</v>
       </c>
-      <c r="D7" s="12">
-        <v>40</v>
-      </c>
-      <c r="E7" s="12">
+      <c r="D7" s="8">
+        <v>42</v>
+      </c>
+      <c r="E7" s="8">
         <v>38</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="J7" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="K7" s="16">
+      <c r="K7" s="12">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="8">
+        <f>(B7-D7)</f>
+        <v>168</v>
+      </c>
+      <c r="C8" s="8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="8">
+        <v>42</v>
+      </c>
+      <c r="E8" s="8">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="8">
+        <f>(B8-D8)</f>
+        <v>126</v>
+      </c>
+      <c r="C9" s="8">
+        <v>3</v>
+      </c>
+      <c r="D9" s="8">
+        <v>42</v>
+      </c>
+      <c r="E9" s="8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="8">
+        <f t="shared" ref="B10:B11" si="0">(B9-D9)</f>
+        <v>84</v>
+      </c>
+      <c r="C10" s="8">
+        <v>4</v>
+      </c>
+      <c r="D10" s="8">
+        <v>42</v>
+      </c>
+      <c r="E10" s="8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="8">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="C11" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12">
-        <f>(B7-D7)</f>
-        <v>157</v>
-      </c>
-      <c r="C8" s="12">
-        <v>2</v>
-      </c>
-      <c r="D8" s="12">
-        <v>40</v>
-      </c>
-      <c r="E8" s="12">
-        <v>31</v>
-      </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="12">
-        <f>(B8-D8)</f>
-        <v>117</v>
-      </c>
-      <c r="C9" s="12">
-        <v>3</v>
-      </c>
-      <c r="D9" s="12">
-        <v>40</v>
-      </c>
-      <c r="E9" s="12">
-        <v>24</v>
-      </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="12">
-        <f t="shared" ref="B10:B11" si="0">(B9-D9)</f>
-        <v>77</v>
-      </c>
-      <c r="C10" s="12">
-        <v>4</v>
-      </c>
-      <c r="D10" s="12">
-        <v>40</v>
-      </c>
-      <c r="E10" s="12">
-        <v>17</v>
-      </c>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="12">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="C11" s="12">
-        <v>5</v>
-      </c>
-      <c r="D11" s="12">
-        <v>37</v>
-      </c>
-      <c r="E11" s="12">
+      <c r="D11" s="8">
+        <v>42</v>
+      </c>
+      <c r="E11" s="8">
         <v>10</v>
       </c>
-      <c r="K11" s="4"/>
     </row>
     <row r="12" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="12">
+      <c r="B12" s="8">
         <v>0</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="8">
         <v>0</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="8">
         <v>3</v>
       </c>
     </row>
@@ -4499,4 +5438,126 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0201B7D8-6E19-4954-984E-425B6655E94F}">
+  <dimension ref="B2:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="17.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="8">
+        <v>2013</v>
+      </c>
+      <c r="C3" s="21">
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="8">
+        <v>2014</v>
+      </c>
+      <c r="C4" s="21">
+        <v>13749542.640000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="8">
+        <v>2015</v>
+      </c>
+      <c r="C5" s="21">
+        <v>15804072</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="8">
+        <v>2016</v>
+      </c>
+      <c r="C6" s="21">
+        <v>18165600</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="8">
+        <v>2017</v>
+      </c>
+      <c r="C7" s="21">
+        <v>20880000</v>
+      </c>
+      <c r="D7" s="19"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="8">
+        <v>2018</v>
+      </c>
+      <c r="C8" s="21">
+        <v>24000000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="8">
+        <v>2019</v>
+      </c>
+      <c r="C9" s="21">
+        <v>27120000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="8">
+        <v>2020</v>
+      </c>
+      <c r="C10" s="21">
+        <v>30645600</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="8">
+        <v>2021</v>
+      </c>
+      <c r="C11" s="21">
+        <v>34629528</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="8">
+        <v>2022</v>
+      </c>
+      <c r="C12" s="21">
+        <v>39131366</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="8">
+        <v>2023</v>
+      </c>
+      <c r="C13" s="21">
+        <v>44218444</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>